<commit_message>
Code is done by Aditya Sonar.It is Commited.
</commit_message>
<xml_diff>
--- a/src/main/resources/testInformation/websitePanel.xlsx
+++ b/src/main/resources/testInformation/websitePanel.xlsx
@@ -3,28 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{30391FC9-F555-4ACB-A00B-B844209656D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C2E5E05D-6FC5-4ED7-980B-DCC211A4C190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="29070" windowHeight="16500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="29100" windowHeight="16500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="IdelMine" sheetId="2" r:id="rId2"/>
+    <sheet name="KlingsStaging" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A7:C39"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -48,10 +39,10 @@
     <t>Y</t>
   </si>
   <si>
-    <t>IdelMine</t>
-  </si>
-  <si>
     <t>UserName</t>
+  </si>
+  <si>
+    <t>KlingsStaging</t>
   </si>
 </sst>
 </file>
@@ -430,7 +421,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -458,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF482862-FE2B-4BD3-8E24-ACCE9DD8ADBE}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A40"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +462,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>